<commit_message>
updated with code block analysis
</commit_message>
<xml_diff>
--- a/docs/FeasibilityAnalysis/MSD2020_FLsImplemented.xlsx
+++ b/docs/FeasibilityAnalysis/MSD2020_FLsImplemented.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20215163\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\FeasibilityAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226F35E4-3689-4572-A887-299B88820A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D5BCF6-9FA5-44DD-8A49-E790DB671D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FLs_Implemented" sheetId="1" r:id="rId1"/>
+    <sheet name="CodeBlocks_Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>Task</t>
   </si>
@@ -178,6 +180,66 @@
   </si>
   <si>
     <t>RuleBook - Law</t>
+  </si>
+  <si>
+    <t>Reference: Integration codes version3 in documents/Design Team</t>
+  </si>
+  <si>
+    <t>Sl No.</t>
+  </si>
+  <si>
+    <t>Code Block</t>
+  </si>
+  <si>
+    <t>Area of Interest</t>
+  </si>
+  <si>
+    <t>Classify teams</t>
+  </si>
+  <si>
+    <t>Create Mask</t>
+  </si>
+  <si>
+    <t>Decision making</t>
+  </si>
+  <si>
+    <t>Detect ball</t>
+  </si>
+  <si>
+    <t>main_task_script</t>
+  </si>
+  <si>
+    <t>zone of field</t>
+  </si>
+  <si>
+    <t>player detection</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>AOI - 3D matrix with information on inner and outer circles separately</t>
+  </si>
+  <si>
+    <t>Player detection output matrix updated with Team A pixel values and Team B pixel values</t>
+  </si>
+  <si>
+    <t>original RGB image returned in maskedRGBImage</t>
+  </si>
+  <si>
+    <t>Number of violators, confidence of violation, centroid of overlapping ara of each detected player with AOI</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>gameState 1-5 (Kickoff, throw in, corner, goal kick, free kick)
+All other players from awarded team are &gt;2m away from ball
+All defenders are &gt;3m away from ball 
+(except one defender in throw in and corner)
+gameState 6 (dropped ball)
+if a player is &lt;1m away from ball, award free kick to opposing team
+determine if all players are &gt;1m away from ball, own penalty area allowed</t>
   </si>
 </sst>
 </file>
@@ -376,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -422,10 +484,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,14 +505,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -725,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F7" sqref="F7:F24"/>
     </sheetView>
   </sheetViews>
@@ -840,17 +912,17 @@
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="14" t="s">
@@ -858,69 +930,69 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="17"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="14" t="s">
@@ -928,69 +1000,69 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="20" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="14" t="s">
@@ -998,51 +1070,51 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="15" t="s">
         <v>27</v>
       </c>
@@ -1128,19 +1200,19 @@
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="14" t="s">
@@ -1148,59 +1220,59 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="14" t="s">
@@ -1208,89 +1280,89 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
       <c r="F39" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
       <c r="F40" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
       <c r="F41" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="20" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="14" t="s">
@@ -1298,77 +1370,91 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
       <c r="F47" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
       <c r="F48" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
       <c r="F49" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
       <c r="F50" s="16" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="C43:C50"/>
+    <mergeCell ref="B43:B50"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="B30:B34"/>
     <mergeCell ref="A43:A50"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B13:B18"/>
@@ -1385,22 +1471,153 @@
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="E43:E50"/>
     <mergeCell ref="D43:D50"/>
-    <mergeCell ref="C43:C50"/>
-    <mergeCell ref="B43:B50"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="D13:D18"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="C13:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A405C9-0149-4D3E-BB84-B6F5374C0F9D}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C747E32B-F1EE-4A2C-AFB3-CA47ED64E6AC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with recommendations and comments
</commit_message>
<xml_diff>
--- a/docs/FeasibilityAnalysis/MSD2020_FLsImplemented.xlsx
+++ b/docs/FeasibilityAnalysis/MSD2020_FLsImplemented.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/probook/Documents/GitHub/AutonomousReferee/AutonomousReferee/docs/FeasibilityAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\FeasibilityAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9740AA-F54F-474D-A9D0-6664A4A6F589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E0DF3C-C16D-4A00-83D8-0795B9F502F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3120" windowWidth="32860" windowHeight="17740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FLs_Implemented" sheetId="1" r:id="rId1"/>
     <sheet name="CodeBlocks_Analysis" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Recommendations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="93">
   <si>
     <t>Task</t>
   </si>
@@ -265,12 +265,69 @@
   <si>
     <t>Slow runtime!</t>
   </si>
+  <si>
+    <t>Decision Making function</t>
+  </si>
+  <si>
+    <t>Player classification</t>
+  </si>
+  <si>
+    <t>Player detection</t>
+  </si>
+  <si>
+    <t>Zone of field</t>
+  </si>
+  <si>
+    <t>Distance violation check (task)</t>
+  </si>
+  <si>
+    <t>Ball detect, locate</t>
+  </si>
+  <si>
+    <t>1.	the code block involves an iteration of the entire image pixel by pixel, which may reduce the speed of the algorithm. There might be faster methods to realize the player detection.
+2.	The code block also has the capability to detect the centers and boundaries of each player. They are not used in the current system, however, it is possible to modify them into output if applicable.</t>
+  </si>
+  <si>
+    <t>Player localization</t>
+  </si>
+  <si>
+    <t>1.The color mask filtering can be made robust to be used for wider range of ball colors.
+2. The robustness of the structuring element used in the morphological operations can be checked.
+Requires manual thresholding based on ball color.</t>
+  </si>
+  <si>
+    <t>The code block involves an iteration of the entire image pixel by pixel, which may reduce the speed of the algorithm. There might be faster methods to realize the player detection. 
+The code block also has the capability to detect the centers and boundaries of each player. They are not used in the current system, however, it is possible to modify them into output if applicable. 
+Assumes players to be 'dark' areas of image. Applies simple centroid computation of region to define player position.</t>
+  </si>
+  <si>
+    <t>Metre-to-pixel ratio could have some uncertainty due to assumption that the field dimensions are ideal (exactly 22 x 14 m). In reality, imperfections in the field dimensions would be overlooked, and this would lead to errors in the calculation  
+Seems fragile and highly influenced by manually-specified field dimensions.</t>
+  </si>
+  <si>
+    <t>Confidence of violation (given to counter the effect of perspective distortion) measure has a trade-off—it could lead to actual violators also being ignored. The reasoning behind using such a confidence measure was that it would be better to have a slightly lenient system that detects gross violations and lets off minor violations than an overly strict system that could lead to unnecessary interruptions in the game.  </t>
+  </si>
+  <si>
+    <t>1.The color mask filtering can be made robust to be used for wider range of player top marker colors.
+2. The robustness of the structuring element used in the morphological operations can be checked.
+The possibility and effectiveness of using other features of the player robots like shape, robot markers and number markers can be looked into. For the current scope, since a top camera was used as the vision system, top markers seemed sensible and has been found to be effective. However, in case of mobile vision systems or side cameras, other features may also need to be used for efficient detection and classification. 
+Distortion correction of the players, especially closer to the penalty area needs to be looked into. In the current scope of work with a top camera, distortion effects were not so prominent. Hence, distortion correction was not looked into much. However, in cases when players of opposite teams are nearby, and their pixels overlap each other due to distortion, there is a possibility of players being classified into the wrong teams in step3 of the algorithm. A possible solution to this problem can be by using distortion correction of the player pixels. Additional Information on the features as discussed in remark 1, or other camera inputs can also be looked into for this problem.</t>
+  </si>
+  <si>
+    <t>1. Although Matlab was chosen because of various reasons, the frequency of the integrated code is slow because of the Matlab implementaion. Other programming languages can be looked into for an increased speed of execution.</t>
+  </si>
+  <si>
+    <t>Task/skill/code block</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +357,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -315,7 +379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -458,11 +522,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -518,26 +666,47 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,17 +994,17 @@
       <selection activeCell="F7" sqref="F7:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="73.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="73.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -855,7 +1024,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -871,7 +1040,7 @@
       </c>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -887,7 +1056,7 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -903,7 +1072,7 @@
       </c>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
@@ -919,7 +1088,7 @@
       </c>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>13</v>
       </c>
@@ -935,215 +1104,215 @@
       </c>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="21"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="24" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="24" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="26"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="26"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>32</v>
       </c>
@@ -1159,7 +1328,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1344,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
@@ -1191,7 +1360,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>36</v>
       </c>
@@ -1207,7 +1376,7 @@
       </c>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>37</v>
       </c>
@@ -1223,248 +1392,262 @@
       </c>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="24" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="26"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="26"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="26"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="26"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
+    <row r="35" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="24" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="24"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
       <c r="F39" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="24"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
       <c r="F40" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="24"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
       <c r="F41" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
       <c r="F42" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
+    <row r="43" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="24" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
       <c r="F44" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
       <c r="F45" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
       <c r="F46" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="24"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
       <c r="F47" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
       <c r="F48" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
       <c r="F49" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
+    <row r="50" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="22"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
       <c r="F50" s="16" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="C43:C50"/>
+    <mergeCell ref="B43:B50"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="B30:B34"/>
     <mergeCell ref="A43:A50"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="B13:B18"/>
@@ -1481,20 +1664,6 @@
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="E43:E50"/>
     <mergeCell ref="D43:D50"/>
-    <mergeCell ref="C43:C50"/>
-    <mergeCell ref="B43:B50"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="D13:D18"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="C13:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1505,25 +1674,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A405C9-0149-4D3E-BB84-B6F5374C0F9D}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.6640625" customWidth="1"/>
-    <col min="5" max="6" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>52</v>
       </c>
@@ -1537,7 +1706,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -1549,7 +1718,7 @@
       </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -1561,7 +1730,7 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -1573,7 +1742,7 @@
       </c>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -1588,7 +1757,7 @@
       </c>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -1602,7 +1771,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>6</v>
       </c>
@@ -1616,7 +1785,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>7</v>
       </c>
@@ -1630,7 +1799,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>8</v>
       </c>
@@ -1652,12 +1821,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C747E32B-F1EE-4A2C-AFB3-CA47ED64E6AC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="129.85546875" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="33">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>8</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>